<commit_message>
nb nn mn n mvv
</commit_message>
<xml_diff>
--- a/Excel/Work schedule.xlsx
+++ b/Excel/Work schedule.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Wake up</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>uiguihihliljl;jknkkllknlk</t>
   </si>
 </sst>
 </file>
@@ -637,37 +640,27 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="10"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="4" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -690,17 +683,27 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="10"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="4" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="6"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -12808,7 +12811,7 @@
   <dimension ref="B1:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -12831,32 +12834,32 @@
     <row r="1" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:14" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="e">
+      <c r="B3" s="42" t="e">
         <f>DAY(DateVal)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="42"/>
       <c r="E3" s="1"/>
       <c r="F3" s="20" t="str">
         <f>IFERROR(UPPER(TEXT(DATE(ReportYear,MonthNumber,ReportDay),"MMMM D, YYYY")),"Invalid Date")</f>
         <v>MARCH 31, 2009</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="L3" s="46" t="s">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="L3" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="46"/>
+      <c r="M3" s="33"/>
       <c r="N3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="E4" s="17">
         <f>'Time Intervals'!B3</f>
         <v>0.25</v>
@@ -12877,16 +12880,16 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A1),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="40" t="s">
+      <c r="M4" s="36" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="E5" s="17">
         <f>'Time Intervals'!B4</f>
         <v>0.27083333333333331</v>
@@ -12895,7 +12898,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="29">
         <v>7</v>
       </c>
       <c r="I5" s="23" t="str">
@@ -12906,12 +12909,12 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A2),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="33"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
       <c r="E6" s="17">
         <f>'Time Intervals'!B5</f>
         <v>0.29166666666666702</v>
@@ -12920,7 +12923,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H6" s="31"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="23" t="str">
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),2),"")</f>
         <v/>
@@ -12929,12 +12932,12 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="33"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="E7" s="17">
         <f>'Time Intervals'!B6</f>
         <v>0.3125</v>
@@ -12955,19 +12958,19 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A4),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L7" s="38" t="s">
+      <c r="L7" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35" t="str">
+      <c r="B8" s="44" t="str">
         <f>TEXT(DateVal,"dddd")</f>
         <v>MARCH 31, 2009</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="44"/>
       <c r="E8" s="17">
         <f>'Time Intervals'!B7</f>
         <v>0.33333333333333298</v>
@@ -12985,12 +12988,12 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A5),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L8" s="38"/>
-      <c r="M8" s="33"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="34"/>
     </row>
     <row r="9" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="E9" s="17">
         <f>'Time Intervals'!B8</f>
         <v>0.35416666666666702</v>
@@ -13008,19 +13011,18 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$7&amp;"|"&amp;ROW(A6),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L9" s="38"/>
-      <c r="M9" s="33"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="34"/>
     </row>
     <row r="10" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
       <c r="E10" s="17">
         <f>'Time Intervals'!B9</f>
         <v>0.375</v>
       </c>
-      <c r="F10" s="18" t="str">
-        <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
-        <v>-</v>
+      <c r="F10" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="H10" s="2" t="e">
         <f>TEXT(DATEVALUE(DateVal)+2,"dddd")</f>
@@ -13034,10 +13036,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A1),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="33"/>
+      <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E11" s="17">
@@ -13048,7 +13050,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="29">
         <v>8</v>
       </c>
       <c r="I11" s="23" t="str">
@@ -13059,8 +13061,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A2),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L11" s="38"/>
-      <c r="M11" s="33"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12" s="17">
@@ -13071,7 +13073,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H12" s="31"/>
+      <c r="H12" s="29"/>
       <c r="I12" s="23" t="str">
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),2),"")</f>
         <v/>
@@ -13080,14 +13082,14 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L12" s="38"/>
-      <c r="M12" s="33"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="34"/>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="43"/>
       <c r="E13" s="17">
         <f>'Time Intervals'!B12</f>
         <v>0.4375</v>
@@ -13108,10 +13110,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A4),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="33"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E14" s="17">
@@ -13131,8 +13133,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A5),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L14" s="38"/>
-      <c r="M14" s="33"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21">
@@ -13158,8 +13160,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$13&amp;"|"&amp;ROW(A6),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="33"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="34"/>
     </row>
     <row r="16" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="8"/>
@@ -13183,10 +13185,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A1),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L16" s="38" t="s">
+      <c r="L16" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="33"/>
+      <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="str">
@@ -13204,7 +13206,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="29">
         <v>9</v>
       </c>
       <c r="I17" s="23" t="str">
@@ -13215,8 +13217,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A2),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L17" s="38"/>
-      <c r="M17" s="33"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
@@ -13231,7 +13233,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H18" s="31"/>
+      <c r="H18" s="29"/>
       <c r="I18" s="23" t="str">
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),2),"")</f>
         <v/>
@@ -13240,8 +13242,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L18" s="38"/>
-      <c r="M18" s="33"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="34"/>
     </row>
     <row r="19" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21">
@@ -13270,10 +13272,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A4),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L19" s="38" t="s">
+      <c r="L19" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="33"/>
+      <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="17">
@@ -13293,8 +13295,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A5),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L20" s="38"/>
-      <c r="M20" s="33"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="17">
@@ -13314,14 +13316,14 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$19&amp;"|"&amp;ROW(A6),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L21" s="38"/>
-      <c r="M21" s="33"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="34"/>
     </row>
     <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="43"/>
       <c r="E22" s="17">
         <f>'Time Intervals'!B21</f>
         <v>0.625</v>
@@ -13342,10 +13344,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$25&amp;"|"&amp;ROW(A1),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L22" s="38" t="s">
+      <c r="L22" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M22" s="33"/>
+      <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E23" s="17">
@@ -13356,7 +13358,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H23" s="31">
+      <c r="H23" s="29">
         <v>10</v>
       </c>
       <c r="I23" s="23" t="str">
@@ -13367,8 +13369,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$25&amp;"|"&amp;ROW(A2),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L23" s="38"/>
-      <c r="M23" s="33"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E24" s="17">
@@ -13379,7 +13381,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H24" s="31"/>
+      <c r="H24" s="29"/>
       <c r="I24" s="23" t="str">
         <f>IFERROR(INDEX(Input[],MATCH($H$25&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),2),"")</f>
         <v/>
@@ -13388,8 +13390,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$25&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L24" s="38"/>
-      <c r="M24" s="33"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="34"/>
     </row>
     <row r="25" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E25" s="17">
@@ -13409,10 +13411,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$25&amp;"|"&amp;ROW(A4),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L25" s="38" t="s">
+      <c r="L25" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M25" s="33"/>
+      <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="17">
@@ -13432,8 +13434,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$25&amp;"|"&amp;ROW(A5),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L26" s="38"/>
-      <c r="M26" s="33"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="34"/>
     </row>
     <row r="27" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="17">
@@ -13456,8 +13458,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$30&amp;"|"&amp;ROW(A1),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L27" s="38"/>
-      <c r="M27" s="33"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="34"/>
     </row>
     <row r="28" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E28" s="17">
@@ -13468,7 +13470,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H28" s="31">
+      <c r="H28" s="29">
         <v>11</v>
       </c>
       <c r="I28" s="23" t="str">
@@ -13479,16 +13481,16 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$30&amp;"|"&amp;ROW(A2),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L28" s="38" t="s">
+      <c r="L28" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M28" s="33"/>
+      <c r="M28" s="34"/>
     </row>
     <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="37"/>
+      <c r="C29" s="46"/>
       <c r="E29" s="17">
         <f>'Time Intervals'!B28</f>
         <v>0.77083333333333304</v>
@@ -13497,7 +13499,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H29" s="31"/>
+      <c r="H29" s="29"/>
       <c r="I29" s="23" t="str">
         <f>IFERROR(INDEX(Input[],MATCH($H$30&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),2),"")</f>
         <v/>
@@ -13506,14 +13508,14 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$30&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L29" s="38"/>
-      <c r="M29" s="33"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="34"/>
     </row>
     <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="30"/>
+      <c r="C30" s="41"/>
       <c r="E30" s="17">
         <f>'Time Intervals'!B29</f>
         <v>0.79166666666666596</v>
@@ -13534,8 +13536,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$30&amp;"|"&amp;ROW(A4),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L30" s="38"/>
-      <c r="M30" s="33"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="34"/>
     </row>
     <row r="31" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E31" s="17">
@@ -13555,10 +13557,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$30&amp;"|"&amp;ROW(A5),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L31" s="38" t="s">
+      <c r="L31" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="M31" s="33"/>
+      <c r="M31" s="34"/>
     </row>
     <row r="32" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="17">
@@ -13581,8 +13583,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$35&amp;"|"&amp;ROW(A1),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L32" s="38"/>
-      <c r="M32" s="33"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="34"/>
     </row>
     <row r="33" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E33" s="17">
@@ -13593,7 +13595,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H33" s="31">
+      <c r="H33" s="29">
         <v>12</v>
       </c>
       <c r="I33" s="23" t="str">
@@ -13604,8 +13606,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$35&amp;"|"&amp;ROW(A2),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L33" s="38"/>
-      <c r="M33" s="33"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E34" s="17">
@@ -13616,7 +13618,7 @@
         <f>IFERROR(INDEX(Input[],MATCH(DATEVALUE(DateVal)&amp;DailySchedule[[#This Row],[Time]],LookUpDateAndTime,0),3),"-")</f>
         <v>-</v>
       </c>
-      <c r="H34" s="31"/>
+      <c r="H34" s="29"/>
       <c r="I34" s="23" t="str">
         <f>IFERROR(INDEX(Input[],MATCH($H$35&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),2),"")</f>
         <v/>
@@ -13625,10 +13627,10 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$35&amp;"|"&amp;ROW(A3),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L34" s="41" t="s">
+      <c r="L34" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="M34" s="33"/>
+      <c r="M34" s="34"/>
     </row>
     <row r="35" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E35" s="17">
@@ -13650,8 +13652,8 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$35&amp;"|"&amp;ROW(A4),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L35" s="42"/>
-      <c r="M35" s="33"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="34"/>
     </row>
     <row r="36" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E36" s="17">
@@ -13671,31 +13673,11 @@
         <f>IFERROR(INDEX(Input[],MATCH($H$35&amp;"|"&amp;ROW(A5),Input[UNIQUE VALUE (CALCULATED)],0),3),"")</f>
         <v/>
       </c>
-      <c r="L36" s="43"/>
-      <c r="M36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="M13:M15"/>
-    <mergeCell ref="M34:M36"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="M10:M12"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="M16:M18"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="L34:L36"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="H33:H34"/>
     <mergeCell ref="B3:C7"/>
@@ -13712,6 +13694,26 @@
     <mergeCell ref="B8:C10"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="L31:L33"/>
+    <mergeCell ref="M34:M36"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="M10:M12"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="M13:M15"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F36">
     <cfRule type="expression" dxfId="8" priority="1">

</xml_diff>